<commit_message>
fix: screenshot for import-map
</commit_message>
<xml_diff>
--- a/__fixtures__/db-screenshot.xlsx
+++ b/__fixtures__/db-screenshot.xlsx
@@ -402,7 +402,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -427,9 +427,12 @@
         <v>mailchimpSetting</v>
       </c>
       <c r="G1" t="str">
+        <v>geoapifySetting</v>
+      </c>
+      <c r="H1" t="str">
         <v>updatedAt</v>
       </c>
-      <c r="H1" t="str">
+      <c r="I1" t="str">
         <v>updatedBy</v>
       </c>
     </row>
@@ -447,12 +450,18 @@
         <v>[{"name":"cheque","hidden":false},{"name":"cash","hidden":false},{"name":"e-transfer","hidden":false}]</v>
       </c>
       <c r="G2" t="str">
-        <v>2025-08-19T13:14:13.341Z</v>
+        <v>{"apiKey":"YZo1n0wIUAVSDBeEsxhgiQ=="}</v>
+      </c>
+      <c r="H2" t="str">
+        <v>2025-08-28T17:37:49.786Z</v>
+      </c>
+      <c r="I2" t="str">
+        <v>dev@email.com</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I2"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
fix: feature overview as gallery (#217)
</commit_message>
<xml_diff>
--- a/__fixtures__/db-screenshot.xlsx
+++ b/__fixtures__/db-screenshot.xlsx
@@ -402,7 +402,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -427,9 +427,12 @@
         <v>mailchimpSetting</v>
       </c>
       <c r="G1" t="str">
+        <v>geoapifySetting</v>
+      </c>
+      <c r="H1" t="str">
         <v>updatedAt</v>
       </c>
-      <c r="H1" t="str">
+      <c r="I1" t="str">
         <v>updatedBy</v>
       </c>
     </row>
@@ -447,12 +450,18 @@
         <v>[{"name":"cheque","hidden":false},{"name":"cash","hidden":false},{"name":"e-transfer","hidden":false}]</v>
       </c>
       <c r="G2" t="str">
-        <v>2025-08-19T13:14:13.341Z</v>
+        <v>{"apiKey":"YZo1n0wIUAVSDBeEsxhgiQ=="}</v>
+      </c>
+      <c r="H2" t="str">
+        <v>2025-08-28T17:37:49.786Z</v>
+      </c>
+      <c r="I2" t="str">
+        <v>dev@email.com</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I2"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>